<commit_message>
functions for processing data
</commit_message>
<xml_diff>
--- a/stations.xlsx
+++ b/stations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muje\Projects\WaterBench-MIKE21SW-SouthernNorthSea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7189ACB-3C21-4593-9BBA-1B31AF3CBFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B8FA98-1A75-494B-835D-F537F15DC686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30690" yWindow="1755" windowWidth="24810" windowHeight="11895" xr2:uid="{232B5731-F377-4082-AC51-0C839DA9EBD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{232B5731-F377-4082-AC51-0C839DA9EBD5}"/>
   </bookViews>
   <sheets>
     <sheet name="stations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
   <si>
     <t>AkkaertSouthwestBuoy</t>
   </si>
@@ -28,9 +28,6 @@
     <t>WaddenEierlandseGat</t>
   </si>
   <si>
-    <t>F16</t>
-  </si>
-  <si>
     <t>F3platform</t>
   </si>
   <si>
@@ -64,12 +61,6 @@
     <t>Latitude</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>AKZ</t>
   </si>
   <si>
@@ -100,15 +91,6 @@
     <t>IJVA</t>
   </si>
   <si>
-    <t>IJVB</t>
-  </si>
-  <si>
-    <t>Ijmuiden Ver A</t>
-  </si>
-  <si>
-    <t>Ijmuiden Ver B</t>
-  </si>
-  <si>
     <t>NWA</t>
   </si>
   <si>
@@ -127,9 +109,6 @@
     <t>Westhinder</t>
   </si>
   <si>
-    <t>Data coverage</t>
-  </si>
-  <si>
     <t>Parameters</t>
   </si>
   <si>
@@ -142,12 +121,6 @@
     <t>RVO/RPS</t>
   </si>
   <si>
-    <t>Hm0, Tz</t>
-  </si>
-  <si>
-    <t>Hm0, TP, Tz, MWD</t>
-  </si>
-  <si>
     <t>Hm0, TP, Tz</t>
   </si>
   <si>
@@ -164,6 +137,54 @@
   </si>
   <si>
     <t>Not on CMEMS</t>
+  </si>
+  <si>
+    <t>VHM0, VTZA</t>
+  </si>
+  <si>
+    <t>VHM0, VTZA, VTPK</t>
+  </si>
+  <si>
+    <t>IJmuidenMunitiestort</t>
+  </si>
+  <si>
+    <t>VHM0, VTZA, VMDR, VTPK</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>KeetenBoei</t>
+  </si>
+  <si>
+    <t>KwintebankBuoy</t>
+  </si>
+  <si>
+    <t>Kwint</t>
+  </si>
+  <si>
+    <t>MaeslantkeringZeezijdeNoordMeetpaal</t>
+  </si>
+  <si>
+    <t>MZ</t>
+  </si>
+  <si>
+    <t>NieuwpoortBuoy</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>Nym</t>
+  </si>
+  <si>
+    <t>Nymindegab</t>
+  </si>
+  <si>
+    <t>Oosterschelde</t>
+  </si>
+  <si>
+    <t>Oost</t>
   </si>
 </sst>
 </file>
@@ -647,10 +668,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1026,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AE3699-4FC1-4F2F-B49F-E90B5736E385}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,50 +1061,43 @@
     <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1">
@@ -1090,364 +1107,461 @@
         <v>2819</v>
       </c>
       <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>51998</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3276</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>54854</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4728</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1">
+        <v>52550</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4058</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>53817</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2950</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>53218</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3220</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>53267</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3633</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1">
+        <v>51608</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3966</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C10" s="1">
+        <v>51349</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2706</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>53277</v>
-      </c>
-      <c r="D3" s="1">
-        <v>4662</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1">
-        <v>51998</v>
-      </c>
-      <c r="D4" s="1">
-        <v>3276</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>63526</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2108</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>54854</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4728</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>53614</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4961</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>51926</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3670</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1">
+        <v>51961</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4159</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>53817</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2950</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>53218</v>
-      </c>
-      <c r="D11" s="1">
-        <v>3220</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1">
-        <v>53267</v>
-      </c>
-      <c r="D12" s="1">
-        <v>3633</v>
-      </c>
-      <c r="F12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1">
-        <v>53614</v>
-      </c>
-      <c r="D13" s="1">
-        <v>4961</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1">
-        <v>51926</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3670</v>
-      </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
       <c r="F15" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="1">
+        <v>51161</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2691</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
       <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="H16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C17" s="1">
+        <v>55810</v>
+      </c>
+      <c r="D17" s="1">
+        <v>7941</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="1">
+        <v>51644</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3481</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1">
         <v>52926</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D19" s="1">
         <v>4151</v>
       </c>
-      <c r="F17" t="s">
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>53277</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4662</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1">
+        <v>513811</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2436</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" t="s">
         <v>38</v>
-      </c>
-      <c r="H17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>